<commit_message>
update ignore file, update reset password
</commit_message>
<xml_diff>
--- a/DataSet/ResetPassword.xlsx
+++ b/DataSet/ResetPassword.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14740" yWindow="460" windowWidth="23660" windowHeight="20000" tabRatio="500"/>
+    <workbookView xWindow="5560" yWindow="1560" windowWidth="27320" windowHeight="14900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Reset Password" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
   <si>
     <t>Internal ID</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Invalid email format</t>
   </si>
   <si>
-    <t>Email is space chars</t>
-  </si>
-  <si>
     <t>Check UI of Reset Password email template</t>
   </si>
   <si>
@@ -77,9 +74,6 @@
     <t>Log out automatically on other devices after user reset password successfully</t>
   </si>
   <si>
-    <t>Open log in page when click on icon</t>
-  </si>
-  <si>
     <t>Can't input over max length in fields</t>
   </si>
   <si>
@@ -98,12 +92,6 @@
     <t>Have emotion/symbol icon in password</t>
   </si>
   <si>
-    <t>The old email still active if have new reset password email</t>
-  </si>
-  <si>
-    <t>Inputting with allow max length (8 to 40 characters)</t>
-  </si>
-  <si>
     <t>Open the home page automatically when user reset pw succussefully</t>
   </si>
   <si>
@@ -164,9 +152,6 @@
     <t>56006</t>
   </si>
   <si>
-    <t>57274</t>
-  </si>
-  <si>
     <t>56022</t>
   </si>
   <si>
@@ -233,7 +218,49 @@
     <t>CONTINUE</t>
   </si>
   <si>
-    <t xml:space="preserve">    </t>
+    <t>Email address place holder</t>
+  </si>
+  <si>
+    <t>Email address</t>
+  </si>
+  <si>
+    <t>Open log in page when click on close icon</t>
+  </si>
+  <si>
+    <t>Reset password with an email which has previously been discarded change</t>
+  </si>
+  <si>
+    <t>Old email when user change email successfully</t>
+  </si>
+  <si>
+    <t>Reset Password with email has invited but hasn't verified yet</t>
+  </si>
+  <si>
+    <t>Reset Password with an email address unverified after change email successfully</t>
+  </si>
+  <si>
+    <t>Reset password an email address which has expired verify email (change email)</t>
+  </si>
+  <si>
+    <t>Have new reset password email</t>
+  </si>
+  <si>
+    <t>Inputting with max allow length (8 to 40 characters)</t>
+  </si>
+  <si>
+    <t>56312</t>
+  </si>
+  <si>
+    <t>56146</t>
+  </si>
+  <si>
+    <t>56144</t>
+  </si>
+  <si>
+    <t>56199</t>
+  </si>
+  <si>
+    <t>56310</t>
   </si>
 </sst>
 </file>
@@ -308,7 +335,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -317,8 +344,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -597,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG32"/>
+  <dimension ref="A1:AG34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -611,6 +637,7 @@
     <col min="6" max="6" width="27.33203125" customWidth="1"/>
     <col min="7" max="7" width="20.5" customWidth="1"/>
     <col min="8" max="8" width="64.1640625" customWidth="1"/>
+    <col min="9" max="9" width="29.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="17" x14ac:dyDescent="0.2">
@@ -633,21 +660,23 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="I1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J1" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
     </row>
     <row r="2" spans="1:33" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
-        <v>39</v>
+      <c r="A2" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -657,15 +686,17 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="J2" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="I2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -691,15 +722,13 @@
       <c r="AG2" s="1"/>
     </row>
     <row r="3" spans="1:33" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
-        <v>40</v>
+      <c r="A3" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>69</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -732,248 +761,294 @@
       <c r="AG3" s="1"/>
     </row>
     <row r="4" spans="1:33" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
-        <v>41</v>
+      <c r="A4" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:33" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
-        <v>42</v>
+      <c r="A5" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:33" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
-        <v>43</v>
+      <c r="A6" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:33" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
-        <v>44</v>
+      <c r="A7" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+        <v>16</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
       <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:33" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
-        <v>45</v>
+      <c r="A8" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:33" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
-        <v>46</v>
+      <c r="A9" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
       <c r="E9" s="4"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:33" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
-        <v>47</v>
+      <c r="A10" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
       <c r="E10" s="4"/>
       <c r="F10" s="6"/>
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:33" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:33" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:33" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:33" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:33" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:33" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:33" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+      <c r="B20" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B21" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:33" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
+    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:33" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:33" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:33" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="9" t="s">
+    <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B26" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-    </row>
-    <row r="32" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>